<commit_message>
fix(test_sheet): test_sheet 세분화 및 보완 [HF-67]
</commit_message>
<xml_diff>
--- a/test_sheet.xlsx
+++ b/test_sheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10511"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81A63A46-83B5-F041-9197-475308C80183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2E4A68A-2D92-C846-8FD3-6E9312C58270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-3440" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="105">
   <si>
     <t>Groceries</t>
   </si>
@@ -487,7 +487,24 @@
 }</t>
   </si>
   <si>
-    <t>1. postman 등을 통해 직접적으로 바꾸지 못하게 변경 시도시 token을 받아와야합니다</t>
+    <t>1. postman 등을 통해 직접적으로 바꾸지 못하게 변경 시도시 Verify 성공시 임시 토큰 등 인증서를 받아와야합니다
+2. 새로운 비밀번호 설정시에도 validation을 확인해야합니다.</t>
+  </si>
+  <si>
+    <t>tmp_token</t>
+  </si>
+  <si>
+    <t>{
+ "userId": "010-3087-0939",
+ "newPassword": "585138",
+ "tmpToken": "qweqwr12345r"
+}</t>
+  </si>
+  <si>
+    <t>(200)
+{
+ "message": "비밀번호가 성공적으로 재설정되었습니다."
+}</t>
   </si>
 </sst>
 </file>
@@ -1623,8 +1640,8 @@
   </sheetPr>
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C12" zoomScale="106" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C5" zoomScale="106" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2441,9 +2458,15 @@
       <c r="G31" s="66" t="s">
         <v>90</v>
       </c>
-      <c r="H31" s="67"/>
-      <c r="I31" s="66"/>
-      <c r="J31" s="66"/>
+      <c r="H31" s="67" t="s">
+        <v>102</v>
+      </c>
+      <c r="I31" s="69" t="s">
+        <v>103</v>
+      </c>
+      <c r="J31" s="69" t="s">
+        <v>104</v>
+      </c>
       <c r="K31" s="66" t="s">
         <v>91</v>
       </c>

</xml_diff>